<commit_message>
Corrections of writing in 1's counter
</commit_message>
<xml_diff>
--- a/Control_Word_Tables_V2.xlsx
+++ b/Control_Word_Tables_V2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="166">
   <si>
     <t>Register</t>
   </si>
@@ -181,12 +181,6 @@
     <t>(data != 0)</t>
   </si>
   <si>
-    <t>R0 &gt;&gt;  → R0</t>
-  </si>
-  <si>
-    <t>Shift R</t>
-  </si>
-  <si>
     <t>S6</t>
   </si>
   <si>
@@ -199,9 +193,6 @@
     <t>1'</t>
   </si>
   <si>
-    <t>R2  →Output Done=1</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -268,12 +259,6 @@
     <t>000</t>
   </si>
   <si>
-    <t>R2  →Output, Done=1</t>
-  </si>
-  <si>
-    <t>xxx,0</t>
-  </si>
-  <si>
     <t>Counter</t>
   </si>
   <si>
@@ -451,15 +436,9 @@
     <t>00001000100010011100</t>
   </si>
   <si>
-    <t>0XXX0010101010011001</t>
-  </si>
-  <si>
     <t>Branch R0!=0</t>
   </si>
   <si>
-    <t>00011XXX0XXXX1000001</t>
-  </si>
-  <si>
     <t>00011001100110010101</t>
   </si>
   <si>
@@ -469,24 +448,9 @@
     <t>0XXXX000100010010000</t>
   </si>
   <si>
-    <t xml:space="preserve">R2  →Output </t>
-  </si>
-  <si>
-    <t>Done=1</t>
-  </si>
-  <si>
-    <t>??REMOVE THE SECOND LOAD</t>
-  </si>
-  <si>
-    <t>#LOAD VALUE TO OUTPUT</t>
-  </si>
-  <si>
     <t>Done=1, OUTPUT ENABLE</t>
   </si>
   <si>
-    <t>0XXX0010101010011000</t>
-  </si>
-  <si>
     <t>XX</t>
   </si>
   <si>
@@ -533,6 +497,33 @@
   </si>
   <si>
     <t>00011001100110000001</t>
+  </si>
+  <si>
+    <t>0---0010101010010001</t>
+  </si>
+  <si>
+    <t>0XXX0010101010010000</t>
+  </si>
+  <si>
+    <t>0XXX0010101010010001</t>
+  </si>
+  <si>
+    <t>R0 &gt;&gt;  0→ R0</t>
+  </si>
+  <si>
+    <t>R0 &gt;&gt;  0 → R0</t>
+  </si>
+  <si>
+    <t>Shift R 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2  →Output  </t>
+  </si>
+  <si>
+    <t>Done=1 output anable</t>
+  </si>
+  <si>
+    <t>Ss7</t>
   </si>
 </sst>
 </file>
@@ -548,18 +539,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -574,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,12 +588,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1229,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
@@ -1268,7 +1247,7 @@
         <v>44</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>26</v>
@@ -1276,25 +1255,25 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="2">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="H14" s="3">
         <v>0</v>
@@ -1315,120 +1294,164 @@
         <v>37</v>
       </c>
       <c r="N14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="2">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="G15" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" s="3">
         <v>0</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I15" s="3">
         <v>0</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H17" s="3">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="3">
+      <c r="O18" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19" s="3">
         <v>0</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>59</v>
+      <c r="O19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -1437,45 +1460,45 @@
         <v>27</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>30</v>
+        <v>141</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>62</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="N20" s="3">
         <v>0</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>26</v>
@@ -1484,381 +1507,232 @@
         <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>26</v>
+        <v>141</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N21" s="3">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>40</v>
+        <v>141</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N22" s="3">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>69</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="2">
-        <v>6</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>50</v>
+        <v>91</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="2">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="2">
-        <v>7</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="2" t="s">
-        <v>143</v>
-      </c>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1871,7 +1745,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1976,10 +1850,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>2</v>
@@ -2011,13 +1885,13 @@
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>34</v>
@@ -2085,7 +1959,7 @@
         <v>37</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2093,7 +1967,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
@@ -2105,10 +1979,10 @@
         <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>26</v>
@@ -2126,10 +2000,10 @@
         <v>44</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2137,7 +2011,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
@@ -2152,7 +2026,7 @@
         <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>26</v>
@@ -2170,10 +2044,10 @@
         <v>44</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2181,7 +2055,7 @@
         <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
@@ -2193,10 +2067,10 @@
         <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>26</v>
@@ -2214,18 +2088,18 @@
         <v>44</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
@@ -2240,7 +2114,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>26</v>
@@ -2255,10 +2129,10 @@
         <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>26</v>
@@ -2266,10 +2140,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
@@ -2281,10 +2155,10 @@
         <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>26</v>
@@ -2302,7 +2176,7 @@
         <v>44</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>26</v>
@@ -2310,25 +2184,25 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>26</v>
@@ -2354,15 +2228,15 @@
     </row>
     <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -2371,45 +2245,45 @@
         <v>26</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -2418,13 +2292,13 @@
         <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>34</v>
@@ -2451,12 +2325,12 @@
         <v>0</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
@@ -2465,13 +2339,13 @@
         <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>40</v>
@@ -2495,245 +2369,245 @@
         <v>37</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="M22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2741,46 +2615,46 @@
         <v>1000</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2792,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,7 +2725,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2859,7 +2733,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2979,19 +2853,19 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>2</v>
@@ -3013,7 +2887,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="Q8" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3027,16 +2901,16 @@
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>26</v>
@@ -3061,7 +2935,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3084,7 +2958,7 @@
         <v>33</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>26</v>
@@ -3093,23 +2967,23 @@
         <v>4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3132,7 +3006,7 @@
         <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>26</v>
@@ -3150,14 +3024,14 @@
         <v>44</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3177,10 +3051,10 @@
         <v>49</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>26</v>
@@ -3195,17 +3069,17 @@
         <v>4</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3219,16 +3093,16 @@
         <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>26</v>
@@ -3253,15 +3127,15 @@
       </c>
       <c r="O13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
@@ -3276,7 +3150,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>26</v>
@@ -3285,28 +3159,28 @@
         <v>4</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O14" s="2"/>
       <c r="Q14" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B15" s="2">
         <v>8</v>
@@ -3324,7 +3198,7 @@
         <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>26</v>
@@ -3339,22 +3213,22 @@
         <v>4</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O15" s="2"/>
       <c r="Q15" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2">
         <v>9</v>
@@ -3363,16 +3237,16 @@
         <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>26</v>
@@ -3390,19 +3264,19 @@
         <v>44</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O16" s="2"/>
       <c r="Q16" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B17" s="8">
         <v>10</v>
@@ -3420,7 +3294,7 @@
         <v>33</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>26</v>
@@ -3435,22 +3309,22 @@
         <v>33</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O17" s="2"/>
       <c r="Q17" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B18" s="2">
         <v>11</v>
@@ -3465,10 +3339,10 @@
         <v>49</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H18" s="8">
         <v>0</v>
@@ -3486,36 +3360,36 @@
         <v>44</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N18" s="8">
         <v>0</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B19" s="1">
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>26</v>
@@ -3540,7 +3414,7 @@
       </c>
       <c r="O19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -3562,12 +3436,12 @@
     </row>
     <row r="21" spans="1:20" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -3581,12 +3455,12 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="8">
         <v>1</v>
@@ -3595,44 +3469,44 @@
         <v>26</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N22" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -3640,7 +3514,7 @@
     </row>
     <row r="23" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" s="8">
         <v>2</v>
@@ -3649,44 +3523,44 @@
         <v>26</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N23" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -3694,7 +3568,7 @@
     </row>
     <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B24" s="8">
         <v>3</v>
@@ -3703,44 +3577,44 @@
         <v>26</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="K24" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -3748,7 +3622,7 @@
     </row>
     <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" s="8">
         <v>4</v>
@@ -3757,44 +3631,44 @@
         <v>26</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -3802,7 +3676,7 @@
     </row>
     <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" s="8">
         <v>5</v>
@@ -3811,44 +3685,44 @@
         <v>26</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N26" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
@@ -3856,7 +3730,7 @@
     </row>
     <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" s="8">
         <v>6</v>
@@ -3865,44 +3739,44 @@
         <v>26</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N27" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -3910,53 +3784,53 @@
     </row>
     <row r="28" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="K28" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N28" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O28" s="8"/>
       <c r="P28" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
@@ -3964,7 +3838,7 @@
     </row>
     <row r="29" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B29" s="8">
         <v>8</v>
@@ -3973,152 +3847,152 @@
         <v>26</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O29" s="8"/>
       <c r="P29" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="12" t="s">
+    <row r="30" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="R30" s="12"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
+      <c r="F30" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
     </row>
     <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N31" s="8" t="s">
         <v>26</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -4126,53 +4000,53 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C32" s="10">
         <v>0</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N32" s="8">
         <v>0</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -4186,46 +4060,46 @@
         <v>12</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H33" s="8">
         <v>0</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N33" s="8" t="s">
         <v>26</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="R33" s="2"/>
     </row>

</xml_diff>